<commit_message>
add the two spider-verse movies
</commit_message>
<xml_diff>
--- a/facts/step3/all-titles.xlsx
+++ b/facts/step3/all-titles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-in-movies\facts\step4-all-films\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-in-movies\facts\step3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{252388BC-041F-458A-B40D-F50485D7A3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD9D6F7-DCD5-4B36-AEAD-E608CDADF0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movies" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="286">
   <si>
     <t>Blade</t>
   </si>
@@ -878,6 +878,24 @@
   </si>
   <si>
     <t>2021–2023</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>Spider-Man: Into the Spider-Verse</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Spider-Man:_Into_the_Spider-Verse</t>
+  </si>
+  <si>
+    <t>spider-verse</t>
+  </si>
+  <si>
+    <t>Spider-Man: Across the Spider-Verse</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Spider-Man:_Across_the_Spider-Verse</t>
   </si>
 </sst>
 </file>
@@ -1230,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1947,17 +1965,17 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
-        <v>2019</v>
+      <c r="A52" s="1" t="s">
+        <v>280</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>281</v>
       </c>
       <c r="C52" t="s">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c r="D52" t="s">
-        <v>122</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1965,10 +1983,10 @@
         <v>2019</v>
       </c>
       <c r="B53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C53" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D53" t="s">
         <v>122</v>
@@ -1979,13 +1997,13 @@
         <v>2019</v>
       </c>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D54" t="s">
-        <v>203</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1993,41 +2011,41 @@
         <v>2019</v>
       </c>
       <c r="B55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D55" t="s">
-        <v>122</v>
+        <v>203</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C56" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D56" t="s">
-        <v>203</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B57" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D57" t="s">
-        <v>122</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -2035,10 +2053,10 @@
         <v>2021</v>
       </c>
       <c r="B58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D58" t="s">
         <v>122</v>
@@ -2049,13 +2067,13 @@
         <v>2021</v>
       </c>
       <c r="B59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C59" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D59" t="s">
-        <v>206</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2063,13 +2081,13 @@
         <v>2021</v>
       </c>
       <c r="B60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D60" t="s">
-        <v>122</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2077,10 +2095,10 @@
         <v>2021</v>
       </c>
       <c r="B61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C61" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D61" t="s">
         <v>122</v>
@@ -2088,16 +2106,16 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C62" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D62" t="s">
-        <v>206</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -2105,13 +2123,13 @@
         <v>2022</v>
       </c>
       <c r="B63" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C63" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D63" t="s">
-        <v>122</v>
+        <v>206</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -2119,10 +2137,10 @@
         <v>2022</v>
       </c>
       <c r="B64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C64" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D64" t="s">
         <v>122</v>
@@ -2133,10 +2151,10 @@
         <v>2022</v>
       </c>
       <c r="B65" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D65" t="s">
         <v>122</v>
@@ -2144,13 +2162,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B66" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C66" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D66" t="s">
         <v>122</v>
@@ -2161,13 +2179,41 @@
         <v>2023</v>
       </c>
       <c r="B67" t="s">
+        <v>63</v>
+      </c>
+      <c r="C67" t="s">
+        <v>272</v>
+      </c>
+      <c r="D67" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>2023</v>
+      </c>
+      <c r="B68" t="s">
         <v>64</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>273</v>
       </c>
-      <c r="D67" t="s">
-        <v>122</v>
+      <c r="D68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B69" t="s">
+        <v>284</v>
+      </c>
+      <c r="C69" t="s">
+        <v>285</v>
+      </c>
+      <c r="D69" t="s">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -2222,22 +2268,22 @@
     <hyperlink ref="B49" r:id="rId48" tooltip="Deadpool 2" display="https://en.wikipedia.org/wiki/Deadpool_2" xr:uid="{5694C499-D8F6-464F-9D3C-676680F5192A}"/>
     <hyperlink ref="B50" r:id="rId49" tooltip="Ant-Man and the Wasp" display="https://en.wikipedia.org/wiki/Ant-Man_and_the_Wasp" xr:uid="{5C7E0751-4553-46D5-989B-C6EB24420260}"/>
     <hyperlink ref="B51" r:id="rId50" tooltip="Venom (2018 film)" display="https://en.wikipedia.org/wiki/Venom_(2018_film)" xr:uid="{0536B05B-7D69-4E63-B0B5-CF14B4483956}"/>
-    <hyperlink ref="B52" r:id="rId51" tooltip="Captain Marvel (film)" display="https://en.wikipedia.org/wiki/Captain_Marvel_(film)" xr:uid="{172F5DB3-3F39-44A1-BA74-1A4CA134053F}"/>
-    <hyperlink ref="B53" r:id="rId52" tooltip="Avengers: Endgame" display="https://en.wikipedia.org/wiki/Avengers:_Endgame" xr:uid="{25C5CAC4-23CC-4380-BDCB-7D4A930A79DF}"/>
-    <hyperlink ref="B54" r:id="rId53" tooltip="Dark Phoenix (film)" display="https://en.wikipedia.org/wiki/Dark_Phoenix_(film)" xr:uid="{7C0ACDBD-F31B-4CAA-8DAC-DA38E78FBBD3}"/>
-    <hyperlink ref="B55" r:id="rId54" tooltip="Spider-Man: Far From Home" display="https://en.wikipedia.org/wiki/Spider-Man:_Far_From_Home" xr:uid="{2AA0861D-7554-4DB9-814E-1C1A87595367}"/>
-    <hyperlink ref="B56" r:id="rId55" tooltip="The New Mutants (film)" display="https://en.wikipedia.org/wiki/The_New_Mutants_(film)" xr:uid="{173967A1-3C9D-4DD7-8E8F-D91235A24945}"/>
-    <hyperlink ref="B57" r:id="rId56" tooltip="Black Widow (2021 film)" display="https://en.wikipedia.org/wiki/Black_Widow_(2021_film)" xr:uid="{51CCC1FC-72FF-4EAC-BF0E-FADD2E5F5ECD}"/>
-    <hyperlink ref="B58" r:id="rId57" tooltip="Shang-Chi and the Legend of the Ten Rings" display="https://en.wikipedia.org/wiki/Shang-Chi_and_the_Legend_of_the_Ten_Rings" xr:uid="{DF698AF0-E4D7-4280-8E3A-FD30CD8383A9}"/>
-    <hyperlink ref="B59" r:id="rId58" tooltip="Venom: Let There Be Carnage" display="https://en.wikipedia.org/wiki/Venom:_Let_There_Be_Carnage" xr:uid="{09DB420E-41D1-4CB8-8F5E-1B1211F8B71E}"/>
-    <hyperlink ref="B60" r:id="rId59" tooltip="Eternals (film)" display="https://en.wikipedia.org/wiki/Eternals_(film)" xr:uid="{F4B33E82-35C8-42C6-AFFB-76469B619C96}"/>
-    <hyperlink ref="B61" r:id="rId60" tooltip="Spider-Man: No Way Home" display="https://en.wikipedia.org/wiki/Spider-Man:_No_Way_Home" xr:uid="{710F600A-565A-40A7-A667-958D283555B0}"/>
-    <hyperlink ref="B62" r:id="rId61" tooltip="Morbius (film)" display="https://en.wikipedia.org/wiki/Morbius_(film)" xr:uid="{8915C02F-A0AF-43F2-8678-987AE231E6DC}"/>
-    <hyperlink ref="B63" r:id="rId62" tooltip="Doctor Strange in the Multiverse of Madness" display="https://en.wikipedia.org/wiki/Doctor_Strange_in_the_Multiverse_of_Madness" xr:uid="{CDBEA5E1-B291-47EA-A287-6F70E8CAB7B1}"/>
-    <hyperlink ref="B64" r:id="rId63" tooltip="Thor: Love and Thunder" display="https://en.wikipedia.org/wiki/Thor:_Love_and_Thunder" xr:uid="{3AB74F2C-F69C-4D2D-BDED-4A813BF8BFEE}"/>
-    <hyperlink ref="B65" r:id="rId64" tooltip="Black Panther: Wakanda Forever" display="https://en.wikipedia.org/wiki/Black_Panther:_Wakanda_Forever" xr:uid="{ADC5FD84-B490-48F8-9C96-439E4409564C}"/>
-    <hyperlink ref="B66" r:id="rId65" tooltip="Ant-Man and the Wasp: Quantumania" display="https://en.wikipedia.org/wiki/Ant-Man_and_the_Wasp:_Quantumania" xr:uid="{B07888B3-15E9-4AFF-902A-DBEAA382600F}"/>
-    <hyperlink ref="B67" r:id="rId66" tooltip="Guardians of the Galaxy Vol. 3" display="https://en.wikipedia.org/wiki/Guardians_of_the_Galaxy_Vol._3" xr:uid="{950701D0-7631-4DC3-B474-8A55F81C297D}"/>
+    <hyperlink ref="B53" r:id="rId51" tooltip="Captain Marvel (film)" display="https://en.wikipedia.org/wiki/Captain_Marvel_(film)" xr:uid="{172F5DB3-3F39-44A1-BA74-1A4CA134053F}"/>
+    <hyperlink ref="B54" r:id="rId52" tooltip="Avengers: Endgame" display="https://en.wikipedia.org/wiki/Avengers:_Endgame" xr:uid="{25C5CAC4-23CC-4380-BDCB-7D4A930A79DF}"/>
+    <hyperlink ref="B55" r:id="rId53" tooltip="Dark Phoenix (film)" display="https://en.wikipedia.org/wiki/Dark_Phoenix_(film)" xr:uid="{7C0ACDBD-F31B-4CAA-8DAC-DA38E78FBBD3}"/>
+    <hyperlink ref="B56" r:id="rId54" tooltip="Spider-Man: Far From Home" display="https://en.wikipedia.org/wiki/Spider-Man:_Far_From_Home" xr:uid="{2AA0861D-7554-4DB9-814E-1C1A87595367}"/>
+    <hyperlink ref="B57" r:id="rId55" tooltip="The New Mutants (film)" display="https://en.wikipedia.org/wiki/The_New_Mutants_(film)" xr:uid="{173967A1-3C9D-4DD7-8E8F-D91235A24945}"/>
+    <hyperlink ref="B58" r:id="rId56" tooltip="Black Widow (2021 film)" display="https://en.wikipedia.org/wiki/Black_Widow_(2021_film)" xr:uid="{51CCC1FC-72FF-4EAC-BF0E-FADD2E5F5ECD}"/>
+    <hyperlink ref="B59" r:id="rId57" tooltip="Shang-Chi and the Legend of the Ten Rings" display="https://en.wikipedia.org/wiki/Shang-Chi_and_the_Legend_of_the_Ten_Rings" xr:uid="{DF698AF0-E4D7-4280-8E3A-FD30CD8383A9}"/>
+    <hyperlink ref="B60" r:id="rId58" tooltip="Venom: Let There Be Carnage" display="https://en.wikipedia.org/wiki/Venom:_Let_There_Be_Carnage" xr:uid="{09DB420E-41D1-4CB8-8F5E-1B1211F8B71E}"/>
+    <hyperlink ref="B61" r:id="rId59" tooltip="Eternals (film)" display="https://en.wikipedia.org/wiki/Eternals_(film)" xr:uid="{F4B33E82-35C8-42C6-AFFB-76469B619C96}"/>
+    <hyperlink ref="B62" r:id="rId60" tooltip="Spider-Man: No Way Home" display="https://en.wikipedia.org/wiki/Spider-Man:_No_Way_Home" xr:uid="{710F600A-565A-40A7-A667-958D283555B0}"/>
+    <hyperlink ref="B63" r:id="rId61" tooltip="Morbius (film)" display="https://en.wikipedia.org/wiki/Morbius_(film)" xr:uid="{8915C02F-A0AF-43F2-8678-987AE231E6DC}"/>
+    <hyperlink ref="B64" r:id="rId62" tooltip="Doctor Strange in the Multiverse of Madness" display="https://en.wikipedia.org/wiki/Doctor_Strange_in_the_Multiverse_of_Madness" xr:uid="{CDBEA5E1-B291-47EA-A287-6F70E8CAB7B1}"/>
+    <hyperlink ref="B65" r:id="rId63" tooltip="Thor: Love and Thunder" display="https://en.wikipedia.org/wiki/Thor:_Love_and_Thunder" xr:uid="{3AB74F2C-F69C-4D2D-BDED-4A813BF8BFEE}"/>
+    <hyperlink ref="B66" r:id="rId64" tooltip="Black Panther: Wakanda Forever" display="https://en.wikipedia.org/wiki/Black_Panther:_Wakanda_Forever" xr:uid="{ADC5FD84-B490-48F8-9C96-439E4409564C}"/>
+    <hyperlink ref="B67" r:id="rId65" tooltip="Ant-Man and the Wasp: Quantumania" display="https://en.wikipedia.org/wiki/Ant-Man_and_the_Wasp:_Quantumania" xr:uid="{B07888B3-15E9-4AFF-902A-DBEAA382600F}"/>
+    <hyperlink ref="B68" r:id="rId66" tooltip="Guardians of the Galaxy Vol. 3" display="https://en.wikipedia.org/wiki/Guardians_of_the_Galaxy_Vol._3" xr:uid="{950701D0-7631-4DC3-B474-8A55F81C297D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId67"/>
@@ -2829,7 +2875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A10" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modify excel, add live action tv series
</commit_message>
<xml_diff>
--- a/facts/step3/all-titles.xlsx
+++ b/facts/step3/all-titles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-in-movies\facts\step3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD9D6F7-DCD5-4B36-AEAD-E608CDADF0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49389F32-6AF4-467E-BAE2-40DDAF4A8C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
   <sheets>
     <sheet name="movies" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="287">
   <si>
     <t>Blade</t>
   </si>
@@ -896,6 +896,9 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Spider-Man:_Across_the_Spider-Verse</t>
+  </si>
+  <si>
+    <t>mcu-netflix</t>
   </si>
 </sst>
 </file>
@@ -1250,8 +1253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEF7CD8B-2C72-4367-8653-A42EAAA710BE}">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2292,10 +2295,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A614F1-7948-4686-8AED-21AFC5640E8C}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2305,11 +2308,10 @@
     <col min="3" max="3" width="56.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.109375" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -2326,13 +2328,10 @@
         <v>121</v>
       </c>
       <c r="F1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2006</v>
       </c>
@@ -2348,11 +2347,11 @@
       <c r="E2">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>69</v>
       </c>
@@ -2368,14 +2367,11 @@
       <c r="E3">
         <v>136</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>71</v>
       </c>
@@ -2391,14 +2387,11 @@
       <c r="E4">
         <v>18</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>72</v>
       </c>
@@ -2414,14 +2407,11 @@
       <c r="E5">
         <v>39</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
@@ -2437,14 +2427,11 @@
       <c r="E6">
         <v>39</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>76</v>
       </c>
@@ -2460,14 +2447,11 @@
       <c r="E7">
         <v>26</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>78</v>
       </c>
@@ -2484,7 +2468,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
@@ -2500,14 +2484,11 @@
       <c r="E9">
         <v>23</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2017</v>
       </c>
@@ -2523,14 +2504,11 @@
       <c r="E10">
         <v>8</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2017</v>
       </c>
@@ -2546,14 +2524,11 @@
       <c r="E11">
         <v>8</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>78</v>
       </c>
@@ -2570,7 +2545,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>78</v>
       </c>
@@ -2586,14 +2561,11 @@
       <c r="E13">
         <v>26</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -2609,14 +2581,11 @@
       <c r="E14">
         <v>33</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>86</v>
       </c>
@@ -2632,14 +2601,11 @@
       <c r="E15">
         <v>20</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2020</v>
       </c>
@@ -2656,7 +2622,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2021</v>
       </c>
@@ -2672,14 +2638,11 @@
       <c r="E17">
         <v>9</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2021</v>
       </c>
@@ -2695,14 +2658,11 @@
       <c r="E18">
         <v>6</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2021</v>
       </c>
@@ -2718,14 +2678,11 @@
       <c r="E19">
         <v>6</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>275</v>
       </c>
@@ -2741,14 +2698,11 @@
       <c r="E20">
         <v>6</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2022</v>
       </c>
@@ -2764,14 +2718,11 @@
       <c r="E21">
         <v>6</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2022</v>
       </c>
@@ -2787,14 +2738,11 @@
       <c r="E22">
         <v>6</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2022</v>
       </c>
@@ -2810,14 +2758,11 @@
       <c r="E23">
         <v>9</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>274</v>
       </c>
@@ -2833,7 +2778,7 @@
       <c r="E24">
         <v>6</v>
       </c>
-      <c r="G24" t="s">
+      <c r="F24" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2875,7 +2820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A10" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add "The Animated Series" to some titles
</commit_message>
<xml_diff>
--- a/facts/step3/all-titles.xlsx
+++ b/facts/step3/all-titles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-in-movies\facts\step3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49389F32-6AF4-467E-BAE2-40DDAF4A8C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F069EA-F0DD-4131-9425-1E305F08EFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="290">
   <si>
     <t>Blade</t>
   </si>
@@ -899,6 +899,15 @@
   </si>
   <si>
     <t>mcu-netflix</t>
+  </si>
+  <si>
+    <t>Spider-Man: The Animated Series</t>
+  </si>
+  <si>
+    <t>X-Men: The Animated Series</t>
+  </si>
+  <si>
+    <t>Fantastic Four: The Animated Series</t>
   </si>
 </sst>
 </file>
@@ -2820,8 +2829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3300BA2F-EA0D-4163-B184-5C04F63CD480}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A10" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2859,7 +2868,7 @@
         <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>288</v>
       </c>
       <c r="C2" t="s">
         <v>164</v>
@@ -2876,7 +2885,7 @@
         <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>289</v>
       </c>
       <c r="C3" t="s">
         <v>165</v>
@@ -2910,7 +2919,7 @@
         <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>287</v>
       </c>
       <c r="C5" t="s">
         <v>167</v>

</xml_diff>

<commit_message>
always use 4 digit year
</commit_message>
<xml_diff>
--- a/facts/step3/all-titles.xlsx
+++ b/facts/step3/all-titles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zhi\Dropbox\Coding\marvelsnap-in-movies\facts\step3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F069EA-F0DD-4131-9425-1E305F08EFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F657AC93-64EE-4AB4-A265-433BF891EC86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{B2277F18-43D7-4F33-8400-65D4D8C9E58A}"/>
   </bookViews>
@@ -247,42 +247,21 @@
     <t>Agents of S.H.I.E.L.D.</t>
   </si>
   <si>
-    <t>2013–20</t>
-  </si>
-  <si>
     <t>Agent Carter</t>
   </si>
   <si>
-    <t>2015–16</t>
-  </si>
-  <si>
-    <t>2015–18</t>
-  </si>
-  <si>
     <t>Jessica Jones</t>
   </si>
   <si>
-    <t>2015–19</t>
-  </si>
-  <si>
     <t>Luke Cage</t>
   </si>
   <si>
-    <t>2016–18</t>
-  </si>
-  <si>
     <t>Legion</t>
   </si>
   <si>
-    <t>2017–19</t>
-  </si>
-  <si>
     <t>Iron Fist</t>
   </si>
   <si>
-    <t>2017–18</t>
-  </si>
-  <si>
     <t>The Defenders</t>
   </si>
   <si>
@@ -298,9 +277,6 @@
     <t>Cloak &amp; Dagger</t>
   </si>
   <si>
-    <t>2018–19</t>
-  </si>
-  <si>
     <t>Helstrom</t>
   </si>
   <si>
@@ -409,18 +385,6 @@
     <t>mcu</t>
   </si>
   <si>
-    <t>1992–97</t>
-  </si>
-  <si>
-    <t>1994–96</t>
-  </si>
-  <si>
-    <t>1994–98</t>
-  </si>
-  <si>
-    <t>1996–97</t>
-  </si>
-  <si>
     <t>Silver Surfer</t>
   </si>
   <si>
@@ -439,45 +403,27 @@
     <t>X-Men: Evolution</t>
   </si>
   <si>
-    <t>2000–03</t>
-  </si>
-  <si>
     <t>Spider-Man: The New Animated Series</t>
   </si>
   <si>
     <t>Fantastic Four: World's Greatest Heroes</t>
   </si>
   <si>
-    <t>2006–07</t>
-  </si>
-  <si>
     <t>The Spectacular Spider-Man</t>
   </si>
   <si>
-    <t>2008–09</t>
-  </si>
-  <si>
     <t>Wolverine and the X-Men</t>
   </si>
   <si>
     <t>Iron Man: Armored Adventures</t>
   </si>
   <si>
-    <t>2009–12</t>
-  </si>
-  <si>
     <t>The Super Hero Squad Show</t>
   </si>
   <si>
-    <t>2009–11</t>
-  </si>
-  <si>
     <t>The Avengers: Earth's Mightiest Heroes</t>
   </si>
   <si>
-    <t>2010–12</t>
-  </si>
-  <si>
     <t>Marvel Anime: Iron Man</t>
   </si>
   <si>
@@ -493,21 +439,12 @@
     <t>Ultimate Spider-Man</t>
   </si>
   <si>
-    <t>2012–17</t>
-  </si>
-  <si>
     <t>Avengers Assemble</t>
   </si>
   <si>
-    <t>2013–19</t>
-  </si>
-  <si>
     <t>Hulk and the Agents of S.M.A.S.H.</t>
   </si>
   <si>
-    <t>2013–15</t>
-  </si>
-  <si>
     <t>Marvel Disk Wars: The Avengers</t>
   </si>
   <si>
@@ -517,9 +454,6 @@
     <t>Marvel's Spider-Man</t>
   </si>
   <si>
-    <t>2017–20</t>
-  </si>
-  <si>
     <t>M.O.D.O.K.</t>
   </si>
   <si>
@@ -625,12 +559,6 @@
     <t>https://en.wikipedia.org/wiki/Moon_Girl_and_Devil_Dinosaur</t>
   </si>
   <si>
-    <t>2010–11</t>
-  </si>
-  <si>
-    <t>2011–12</t>
-  </si>
-  <si>
     <t>2017</t>
   </si>
   <si>
@@ -865,9 +793,6 @@
     <t>2023</t>
   </si>
   <si>
-    <t>2021–24</t>
-  </si>
-  <si>
     <t>isAnime</t>
   </si>
   <si>
@@ -908,6 +833,81 @@
   </si>
   <si>
     <t>Fantastic Four: The Animated Series</t>
+  </si>
+  <si>
+    <t>2000–2003</t>
+  </si>
+  <si>
+    <t>2006–2007</t>
+  </si>
+  <si>
+    <t>2008–2009</t>
+  </si>
+  <si>
+    <t>2009–2012</t>
+  </si>
+  <si>
+    <t>2009–2011</t>
+  </si>
+  <si>
+    <t>2010–2012</t>
+  </si>
+  <si>
+    <t>2010–2011</t>
+  </si>
+  <si>
+    <t>2011–2012</t>
+  </si>
+  <si>
+    <t>2012–2017</t>
+  </si>
+  <si>
+    <t>2013–2019</t>
+  </si>
+  <si>
+    <t>2013–2015</t>
+  </si>
+  <si>
+    <t>2015–2016</t>
+  </si>
+  <si>
+    <t>2015–2019</t>
+  </si>
+  <si>
+    <t>2017–2018</t>
+  </si>
+  <si>
+    <t>2017–2020</t>
+  </si>
+  <si>
+    <t>2013–2020</t>
+  </si>
+  <si>
+    <t>2015–2018</t>
+  </si>
+  <si>
+    <t>2016–2018</t>
+  </si>
+  <si>
+    <t>2017–2019</t>
+  </si>
+  <si>
+    <t>2018–2019</t>
+  </si>
+  <si>
+    <t>2021–2024</t>
+  </si>
+  <si>
+    <t>1992–1997</t>
+  </si>
+  <si>
+    <t>1994–1996</t>
+  </si>
+  <si>
+    <t>1994–1998</t>
+  </si>
+  <si>
+    <t>1996–1997</t>
   </si>
 </sst>
 </file>
@@ -1282,10 +1282,10 @@
         <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="D1" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1296,10 +1296,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="D2" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1310,10 +1310,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
       <c r="D3" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1324,10 +1324,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="D4" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1338,10 +1338,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="D5" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1352,10 +1352,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1366,10 +1366,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="D7" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1380,7 +1380,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1391,7 +1391,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1402,10 +1402,10 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="D10" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1416,10 +1416,10 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="D11" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1430,10 +1430,10 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
       <c r="D12" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1444,10 +1444,10 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="D13" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1458,10 +1458,10 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="D14" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1472,10 +1472,10 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
       <c r="D15" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1486,10 +1486,10 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1500,10 +1500,10 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="D17" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1514,10 +1514,10 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1528,10 +1528,10 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="D19" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1542,7 +1542,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1553,10 +1553,10 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="D21" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1567,10 +1567,10 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1581,10 +1581,10 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="D23" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1595,10 +1595,10 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="D24" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1609,10 +1609,10 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="D25" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1623,10 +1623,10 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="D26" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1637,10 +1637,10 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="D27" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1651,10 +1651,10 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="D28" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1665,10 +1665,10 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="D29" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1679,10 +1679,10 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
       <c r="D30" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1693,10 +1693,10 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="D31" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1707,10 +1707,10 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1721,10 +1721,10 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
       <c r="D33" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1735,10 +1735,10 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="D34" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1749,10 +1749,10 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="D35" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1763,10 +1763,10 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
       <c r="D36" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1777,10 +1777,10 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="D37" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1791,7 +1791,7 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1802,10 +1802,10 @@
         <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
       <c r="D39" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1816,10 +1816,10 @@
         <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="D40" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1830,10 +1830,10 @@
         <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="D41" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1844,10 +1844,10 @@
         <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
       <c r="D42" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1858,10 +1858,10 @@
         <v>40</v>
       </c>
       <c r="C43" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="D43" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1872,10 +1872,10 @@
         <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="D44" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1886,24 +1886,24 @@
         <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="D45" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
       <c r="B46" t="s">
         <v>43</v>
       </c>
       <c r="C46" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="D46" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1914,10 +1914,10 @@
         <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="D47" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1928,10 +1928,10 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
       <c r="D48" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1942,10 +1942,10 @@
         <v>46</v>
       </c>
       <c r="C49" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="D49" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1956,10 +1956,10 @@
         <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="D50" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1970,24 +1970,24 @@
         <v>48</v>
       </c>
       <c r="C51" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="D51" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="B52" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="C52" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
       <c r="D52" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1998,10 +1998,10 @@
         <v>49</v>
       </c>
       <c r="C53" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="D53" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -2012,10 +2012,10 @@
         <v>50</v>
       </c>
       <c r="C54" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="D54" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -2026,10 +2026,10 @@
         <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="D55" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -2040,10 +2040,10 @@
         <v>52</v>
       </c>
       <c r="C56" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="D56" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -2054,10 +2054,10 @@
         <v>53</v>
       </c>
       <c r="C57" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="D57" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -2068,10 +2068,10 @@
         <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="D58" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -2082,10 +2082,10 @@
         <v>55</v>
       </c>
       <c r="C59" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="D59" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2096,10 +2096,10 @@
         <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="D60" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2110,10 +2110,10 @@
         <v>57</v>
       </c>
       <c r="C61" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="D61" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -2124,10 +2124,10 @@
         <v>58</v>
       </c>
       <c r="C62" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="D62" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -2138,10 +2138,10 @@
         <v>59</v>
       </c>
       <c r="C63" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="D63" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -2152,10 +2152,10 @@
         <v>60</v>
       </c>
       <c r="C64" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="D64" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2166,10 +2166,10 @@
         <v>61</v>
       </c>
       <c r="C65" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="D65" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -2180,10 +2180,10 @@
         <v>62</v>
       </c>
       <c r="C66" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="D66" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -2194,10 +2194,10 @@
         <v>63</v>
       </c>
       <c r="C67" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
       <c r="D67" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -2208,24 +2208,24 @@
         <v>64</v>
       </c>
       <c r="C68" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="D68" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="B69" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="C69" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
       <c r="D69" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2307,7 +2307,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2328,16 +2328,16 @@
         <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F1" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2348,7 +2348,7 @@
         <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2357,18 +2357,18 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>280</v>
       </c>
       <c r="B3" t="s">
         <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D3">
         <v>7</v>
@@ -2377,18 +2377,18 @@
         <v>136</v>
       </c>
       <c r="F3" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>71</v>
+        <v>276</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -2397,18 +2397,18 @@
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>72</v>
+        <v>281</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -2417,18 +2417,18 @@
         <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>74</v>
+        <v>277</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -2437,18 +2437,18 @@
         <v>39</v>
       </c>
       <c r="F6" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>282</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -2457,18 +2457,18 @@
         <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>78</v>
+        <v>283</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -2479,13 +2479,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>80</v>
+        <v>278</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -2494,7 +2494,7 @@
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -2502,10 +2502,10 @@
         <v>2017</v>
       </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2514,7 +2514,7 @@
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -2522,10 +2522,10 @@
         <v>2017</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C11" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2534,18 +2534,18 @@
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>78</v>
+        <v>283</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -2556,13 +2556,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>78</v>
+        <v>283</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -2571,18 +2571,18 @@
         <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>78</v>
+        <v>283</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -2591,18 +2591,18 @@
         <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>86</v>
+        <v>284</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -2611,7 +2611,7 @@
         <v>20</v>
       </c>
       <c r="F15" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2619,10 +2619,10 @@
         <v>2020</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2636,10 +2636,10 @@
         <v>2021</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C17" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2648,7 +2648,7 @@
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2656,10 +2656,10 @@
         <v>2021</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -2668,7 +2668,7 @@
         <v>6</v>
       </c>
       <c r="F18" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -2676,10 +2676,10 @@
         <v>2021</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -2688,18 +2688,18 @@
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2708,7 +2708,7 @@
         <v>6</v>
       </c>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2716,10 +2716,10 @@
         <v>2022</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2728,7 +2728,7 @@
         <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2736,10 +2736,10 @@
         <v>2022</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C22" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2748,7 +2748,7 @@
         <v>6</v>
       </c>
       <c r="F22" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2756,10 +2756,10 @@
         <v>2022</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -2768,18 +2768,18 @@
         <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -2788,7 +2788,7 @@
         <v>6</v>
       </c>
       <c r="F24" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2830,7 +2830,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2851,27 +2851,27 @@
         <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F1" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>123</v>
+        <v>286</v>
       </c>
       <c r="B2" t="s">
-        <v>288</v>
+        <v>263</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -2882,13 +2882,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>124</v>
+        <v>287</v>
       </c>
       <c r="B3" t="s">
-        <v>289</v>
+        <v>264</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -2899,13 +2899,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>124</v>
+        <v>287</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -2916,13 +2916,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>125</v>
+        <v>288</v>
       </c>
       <c r="B5" t="s">
-        <v>287</v>
+        <v>262</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -2933,13 +2933,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>126</v>
+        <v>289</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -2953,10 +2953,10 @@
         <v>1998</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2967,13 +2967,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2984,13 +2984,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -3001,13 +3001,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>133</v>
+        <v>265</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -3021,10 +3021,10 @@
         <v>2003</v>
       </c>
       <c r="B11" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>173</v>
+        <v>151</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -3035,13 +3035,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>136</v>
+        <v>266</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -3052,13 +3052,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>138</v>
+        <v>267</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C13" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -3072,10 +3072,10 @@
         <v>2009</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -3086,13 +3086,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>141</v>
+        <v>268</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>177</v>
+        <v>155</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -3103,13 +3103,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>143</v>
+        <v>269</v>
       </c>
       <c r="B16" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C16" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -3120,13 +3120,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>145</v>
+        <v>270</v>
       </c>
       <c r="B17" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="C17" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -3137,13 +3137,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>195</v>
+        <v>271</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="C18" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -3152,18 +3152,18 @@
         <v>12</v>
       </c>
       <c r="F18" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>196</v>
+        <v>272</v>
       </c>
       <c r="B19" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -3172,18 +3172,18 @@
         <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>196</v>
+        <v>272</v>
       </c>
       <c r="B20" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="C20" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -3192,18 +3192,18 @@
         <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>196</v>
+        <v>272</v>
       </c>
       <c r="B21" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="C21" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -3212,18 +3212,18 @@
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>151</v>
+        <v>273</v>
       </c>
       <c r="B22" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="D22">
         <v>4</v>
@@ -3234,13 +3234,13 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>153</v>
+        <v>274</v>
       </c>
       <c r="B23" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="C23" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="D23">
         <v>5</v>
@@ -3251,13 +3251,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>155</v>
+        <v>275</v>
       </c>
       <c r="B24" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="C24" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -3268,13 +3268,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>71</v>
+        <v>276</v>
       </c>
       <c r="B25" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="C25" t="s">
-        <v>187</v>
+        <v>165</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -3283,18 +3283,18 @@
         <v>51</v>
       </c>
       <c r="F25" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>277</v>
       </c>
       <c r="B26" t="s">
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -3305,13 +3305,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>80</v>
+        <v>278</v>
       </c>
       <c r="B27" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="C27" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="D27">
         <v>2</v>
@@ -3320,18 +3320,18 @@
         <v>39</v>
       </c>
       <c r="F27" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>159</v>
+        <v>279</v>
       </c>
       <c r="B28" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="C28" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -3345,10 +3345,10 @@
         <v>2021</v>
       </c>
       <c r="B29" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="C29" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -3359,13 +3359,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
       <c r="B30" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="C30" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -3376,13 +3376,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="B31" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="C31" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -3393,13 +3393,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="B32" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="C32" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="D32">
         <v>1</v>

</xml_diff>